<commit_message>
Badge number search, other bug fixed
</commit_message>
<xml_diff>
--- a/public/34pass-heretomeet.xlsx
+++ b/public/34pass-heretomeet.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="heretomeet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,23 +48,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>sr #</t>
+    <t>name</t>
   </si>
   <si>
-    <t>mobile number</t>
+    <t>mobile_number</t>
   </si>
   <si>
-    <t>email address</t>
+    <t>email</t>
   </si>
   <si>
-    <t>name</t>
+    <t>badge_nubmer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +77,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,13 +104,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,26 +405,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -417,8 +434,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="D2" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>